<commit_message>
fix input question must have at least 2 words
</commit_message>
<xml_diff>
--- a/train001.xlsx
+++ b/train001.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6400" yWindow="460" windowWidth="25600" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -993,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>